<commit_message>
added smcl for sulfate to plots 8 and 9
</commit_message>
<xml_diff>
--- a/data/biweekly/ccbor-biweekly-stolz.xlsx
+++ b/data/biweekly/ccbor-biweekly-stolz.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2185" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2185" uniqueCount="296">
   <si>
     <t xml:space="preserve">site</t>
   </si>
@@ -889,6 +889,27 @@
   </si>
   <si>
     <t xml:space="preserve">Ti (mg/L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fe (mg/L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methane (ppb)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethane (ppb)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethene (ppb)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Propane (ppb)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Propylene (ppb)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Butane (ppb)</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1072,7 @@
       <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.52"/>
@@ -1079,7 +1100,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="8.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="6.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="10.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="7.26"/>
@@ -1108,7 +1129,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="70" style="0" width="7.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="72" min="72" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="72" min="72" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="73" style="0" width="9.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="0" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="0" width="12.41"/>
@@ -17457,7 +17478,7 @@
       <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="37.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.06"/>
@@ -18475,16 +18496,16 @@
   </sheetPr>
   <dimension ref="A1:BM37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AT1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BM4" activeCellId="0" sqref="BM4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.1"/>
@@ -18499,7 +18520,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="8.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="6.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="7.26"/>
@@ -18528,7 +18549,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="60" style="0" width="7.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="0" width="9.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="0" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="0" width="12.41"/>
@@ -18650,7 +18671,7 @@
         <v>47</v>
       </c>
       <c r="AM1" s="8" t="s">
-        <v>48</v>
+        <v>289</v>
       </c>
       <c r="AN1" s="8" t="s">
         <v>49</v>
@@ -18710,22 +18731,22 @@
         <v>67</v>
       </c>
       <c r="BG1" s="8" t="s">
-        <v>68</v>
+        <v>290</v>
       </c>
       <c r="BH1" s="8" t="s">
-        <v>69</v>
+        <v>291</v>
       </c>
       <c r="BI1" s="8" t="s">
-        <v>70</v>
+        <v>292</v>
       </c>
       <c r="BJ1" s="8" t="s">
-        <v>71</v>
+        <v>293</v>
       </c>
       <c r="BK1" s="8" t="s">
-        <v>72</v>
+        <v>294</v>
       </c>
       <c r="BL1" s="8" t="s">
-        <v>73</v>
+        <v>295</v>
       </c>
       <c r="BM1" s="8"/>
     </row>

</xml_diff>

<commit_message>
corrected site 9 in mean std table biweekly
</commit_message>
<xml_diff>
--- a/data/biweekly/ccbor-biweekly-stolz.xlsx
+++ b/data/biweekly/ccbor-biweekly-stolz.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="ccbor-biweekly-stolz" sheetId="1" state="visible" r:id="rId2"/>
@@ -1068,11 +1068,11 @@
   </sheetPr>
   <dimension ref="A1:BW221"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AE1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E196" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D198" activeCellId="0" sqref="198:198"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.52"/>
@@ -17474,11 +17474,11 @@
   </sheetPr>
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M11" activeCellId="1" sqref="198:198 M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="37.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.06"/>
@@ -17545,7 +17545,7 @@
         <v>458</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>798</v>
+        <v>1612</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>8</v>
@@ -17592,7 +17592,7 @@
         <v>458</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>534</v>
+        <v>1089</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>250</v>
@@ -17640,7 +17640,7 @@
         <v>513</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>854</v>
+        <v>1696</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>251</v>
@@ -17691,7 +17691,7 @@
         <v>434</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>805</v>
+        <v>1606</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>252</v>
@@ -17742,7 +17742,7 @@
         <v>481</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>791</v>
+        <v>1582</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>253</v>
@@ -17793,7 +17793,7 @@
         <v>418</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>679</v>
+        <v>1372</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>254</v>
@@ -17844,7 +17844,7 @@
         <v>328</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>398</v>
+        <v>816</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>255</v>
@@ -17895,7 +17895,7 @@
         <v>376</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>647</v>
+        <v>1287</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>256</v>
@@ -17946,7 +17946,7 @@
         <v>358</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>554</v>
+        <v>1135</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>257</v>
@@ -17997,26 +17997,26 @@
         <v>235</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>213</v>
+        <v>451</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>258</v>
       </c>
       <c r="M11" s="6" t="n">
         <f aca="false">AVERAGE(J2:J26)</f>
-        <v>546.791666666667</v>
+        <v>1107.45833333333</v>
       </c>
       <c r="N11" s="4" t="n">
         <f aca="false">MIN(J2:J26)</f>
-        <v>130</v>
+        <v>275</v>
       </c>
       <c r="O11" s="4" t="n">
         <f aca="false">MAX(J2:J26)</f>
-        <v>854</v>
+        <v>1696</v>
       </c>
       <c r="P11" s="7" t="n">
         <f aca="false">STDEV(J2:J26)</f>
-        <v>224.786271274789</v>
+        <v>444.835776161971</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18048,7 +18048,7 @@
         <v>316</v>
       </c>
       <c r="J12" s="0" t="n">
-        <v>569</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18080,7 +18080,7 @@
         <v>368</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>684</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18109,7 +18109,7 @@
         <v>376</v>
       </c>
       <c r="J14" s="0" t="n">
-        <v>426</v>
+        <v>788</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18138,7 +18138,7 @@
         <v>335</v>
       </c>
       <c r="J15" s="0" t="n">
-        <v>323</v>
+        <v>669</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18170,7 +18170,7 @@
         <v>277</v>
       </c>
       <c r="J16" s="0" t="n">
-        <v>446</v>
+        <v>955</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18202,7 +18202,7 @@
         <v>254</v>
       </c>
       <c r="J17" s="0" t="n">
-        <v>418</v>
+        <v>878</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18234,7 +18234,7 @@
         <v>395</v>
       </c>
       <c r="J18" s="0" t="n">
-        <v>762</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18266,7 +18266,7 @@
         <v>350</v>
       </c>
       <c r="J19" s="0" t="n">
-        <v>553</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18298,7 +18298,7 @@
         <v>194</v>
       </c>
       <c r="J20" s="0" t="n">
-        <v>159</v>
+        <v>333</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18330,7 +18330,7 @@
         <v>182</v>
       </c>
       <c r="J21" s="0" t="n">
-        <v>780</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18362,7 +18362,7 @@
         <v>342</v>
       </c>
       <c r="J22" s="0" t="n">
-        <v>130</v>
+        <v>275</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18394,7 +18394,7 @@
         <v>653</v>
       </c>
       <c r="J23" s="0" t="n">
-        <v>707</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18426,7 +18426,7 @@
         <v>306</v>
       </c>
       <c r="J24" s="0" t="n">
-        <v>186</v>
+        <v>391</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18458,7 +18458,7 @@
         <v>570</v>
       </c>
       <c r="J25" s="0" t="n">
-        <v>707</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18496,11 +18496,11 @@
   </sheetPr>
   <dimension ref="A1:BM37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AT1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BM4" activeCellId="0" sqref="BM4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AT1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BM4" activeCellId="1" sqref="198:198 BM4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.52"/>

</xml_diff>